<commit_message>
updated Sprint Plan to reflect Sprint 2 goals, daily Burndown Chart update
</commit_message>
<xml_diff>
--- a/Sprint Documentation/Burndown Chart Caliber Mobile.xlsx
+++ b/Sprint Documentation/Burndown Chart Caliber Mobile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Burndown Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Sprint Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AA66D9-0622-497E-AB3F-75F49DC9E6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933903AB-13F4-4343-91FE-133D3DEAE9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
@@ -470,6 +470,9 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
@@ -1052,6 +1055,9 @@
                 <c:pt idx="7">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2734,7 +2740,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2849,6 +2855,9 @@
       </c>
       <c r="B10">
         <v>13</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated burndown chart, updated skeleton presentation
</commit_message>
<xml_diff>
--- a/Sprint Documentation/Burndown Chart Caliber Mobile.xlsx
+++ b/Sprint Documentation/Burndown Chart Caliber Mobile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Sprint Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25FB9AE-4DF1-4AB1-8216-08A6E10930B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2178C0-A54A-4C3A-826E-C52604C31FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
@@ -323,7 +323,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
@@ -477,6 +477,27 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,7 +930,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
@@ -1063,6 +1084,27 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2746,7 +2788,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2884,6 +2926,9 @@
       <c r="B12">
         <v>13</v>
       </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -2892,6 +2937,9 @@
       <c r="B13">
         <v>13</v>
       </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -2900,13 +2948,19 @@
       <c r="B14">
         <v>13</v>
       </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44417</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -2916,6 +2970,9 @@
       <c r="B16">
         <v>5</v>
       </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -2924,6 +2981,9 @@
       <c r="B17">
         <v>5</v>
       </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -2931,6 +2991,9 @@
       </c>
       <c r="B18">
         <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>